<commit_message>
Changed Anforderungen.xlsx Removed Anforderungen_Steffen.xls
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Nichtfunktionale Anforderungen" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Funktionale Anforderungen'!$A$1:$E$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Funktionale Anforderungen'!$A$1:$E$22</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
   <si>
     <t>Feature</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Benutzerverwaltung</t>
   </si>
   <si>
-    <t>Eintragen was man teilen möchte, Beschreibung, Ausleihdauer</t>
-  </si>
-  <si>
     <t>Mängelbeschreibung</t>
   </si>
   <si>
@@ -191,12 +188,6 @@
     <t>Als Betreiber möchte ich einen Haftungsausschluss, um mich gegen rechtliche Klagen von Nutzern im Bezug auf die Anwendung abzusichern.</t>
   </si>
   <si>
-    <t>Bei jedem Gegendstand soll ein Status anzeigt werden, ob er verfügbar ist oder nicht</t>
-  </si>
-  <si>
-    <t>Als Ausleihender möchte ich eine Statusanzeige um zu erkennen ob der gewünscht Gegenstand verfügbar ist. Als Verleihender möchte ich eine Statusanzeige um Dinge die ich zurzeit selbst benötige vom Verleih auszuschließen</t>
-  </si>
-  <si>
     <t>Aus Ausleihender möchte ich eine Restzeitanzeige um zu wissen wann ein Gegendstand wieder zum Verleih bereit steht</t>
   </si>
   <si>
@@ -216,13 +207,67 @@
   </si>
   <si>
     <t>Als Facebook Nutzer möchte ich den Facebook-Login um mich mit meinem vorhanden Facebook Konto bei dir Anwendung zu authentifieren</t>
+  </si>
+  <si>
+    <t>Gegenstände zum Verleih freigeben</t>
+  </si>
+  <si>
+    <t>Gegenstände eintragen die man verleihen möchte. Die Gegenstände können beschrieben werden, Bilder hinzugefügt werden und eine Ausleihdauer bestimmt werden.</t>
+  </si>
+  <si>
+    <t>Gegenstand in eine Kategorie (z.B. Kleidung) einordnen</t>
+  </si>
+  <si>
+    <t>Aus einer vorgegebenen Liste von Kategorien eine Kategorie auswählen, die zu dem Gegenstand, der verliehen wird, passt.</t>
+  </si>
+  <si>
+    <t>Jeder User bekommt einen Eigenen Account in dem die wichtigsten Inos über Ihn stehen.</t>
+  </si>
+  <si>
+    <t>Bei der ersten Anmeldung muss ein Account angelegt werden, der aus Name, PWD und andere wichtige Infos besteht. Man kann sich an- und abmelden und sein Profil nachträglich bearbeiten.</t>
+  </si>
+  <si>
+    <t>Verfügbaren Gegenstände können ausgeliehen werden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein verfügbarer Gegenstand kann zum Ausleihen ausgewählt werden. Der Ausleiher bekommt darauf hin eine Anfrage, dass diese Person diesen Gegenstand ausleihen möchte. Der Ausleiher kann die Anfrage annehmen oder ablehnen. Bei positiver bestätigung bekommt die Person die Daten des Ausleihers. </t>
+  </si>
+  <si>
+    <t>Nach einem bestimmten Gegenstand kann gesucht werden</t>
+  </si>
+  <si>
+    <t>Den Name des Gegenstands, den man ausleihen möchte, kann man in ein Suchfeld eingeben und dann danach Suchen. Gegenstände in der nähe mit ähnlichen Namen werden darauf hin angezeigt</t>
+  </si>
+  <si>
+    <t>Nach einem Benutzer kann gesucht werden</t>
+  </si>
+  <si>
+    <t>Den Namen eines Benutzer kann in ein Suchfeld eingegeben werden und anschließend danach gesucht werden. Benutzer mit ähnlichen Namen werden angezeigt. Bei Auswahl eines Benutzer, wird das Profil angezeigt.</t>
+  </si>
+  <si>
+    <t>Gegenstand Suche</t>
+  </si>
+  <si>
+    <t>Must-be</t>
+  </si>
+  <si>
+    <t>Benutzer suche</t>
+  </si>
+  <si>
+    <t>Nice-to-have</t>
+  </si>
+  <si>
+    <t>Mängel, die ein Gegenstand hat, können bei der Beschreibung des Gegenstandes eingegeben werden</t>
+  </si>
+  <si>
+    <t>Auf der Seite des Gegenstandes können vom Verleiher und Personen, die den Gegenstand kürzlich ausgeliehen haben in einem extra Feld angegeben werden.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +282,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -256,17 +308,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -569,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,299 +652,351 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" t="s">
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" t="s">
+      <c r="C11" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" t="s">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" t="s">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" t="s">
+      <c r="C19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" t="s">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" t="s">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" t="s">
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" t="s">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E20"/>
+  <autoFilter ref="A1:E22"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -919,116 +1029,116 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Anforderungen.xlsx Updated Anwesenheitsliste.xlsx
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -4,22 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18516" windowHeight="4944"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18510" windowHeight="4950"/>
   </bookViews>
   <sheets>
     <sheet name="Funktionale Anforderungen" sheetId="1" r:id="rId1"/>
     <sheet name="Nichtfunktionale Anforderungen" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Funktionale Anforderungen'!$A$1:$E$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Funktionale Anforderungen'!$A$1:$F$22</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="105">
   <si>
     <t>Feature</t>
   </si>
@@ -174,9 +173,6 @@
     <t>Als Nutzer möchte ich meine persönlichen Informationen angeben und die anderer Nutzer einsehen können, um schneller eine Transaktion ausführen zu können.</t>
   </si>
   <si>
-    <t>Als Nutzer möchte ich Produkte melden können</t>
-  </si>
-  <si>
     <t>Als Nutzer möchte ich Benutzer melden können, um im Falle eines Verstoßes gegen den Verhaltenskodex diesen Nutzer bestrafen zu lassen, damit alle ein positives Erlebnis mit der Anwendung haben</t>
   </si>
   <si>
@@ -225,9 +221,6 @@
     <t>Jeder User bekommt einen Eigenen Account in dem die wichtigsten Inos über Ihn stehen.</t>
   </si>
   <si>
-    <t>Bei der ersten Anmeldung muss ein Account angelegt werden, der aus Name, PWD und andere wichtige Infos besteht. Man kann sich an- und abmelden und sein Profil nachträglich bearbeiten.</t>
-  </si>
-  <si>
     <t>Verfügbaren Gegenstände können ausgeliehen werden</t>
   </si>
   <si>
@@ -322,6 +315,24 @@
   </si>
   <si>
     <t>Der nutzer bekommt nachrichten über Artikeln.</t>
+  </si>
+  <si>
+    <t>Als Ausleihender möchte ich eine Statusanzeige um zu erkennen ob der gewünscht Gegenstand verfügbar ist. Als Verleihender möchte ich eine Statusanzeige um Dinge die ich zurzeit selbst benötige vom Verleih auszuschließen</t>
+  </si>
+  <si>
+    <t>Anzeige ob Produkt verfügbar oder nicht</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Bei der ersten Anmeldung muss ein Account angelegt werden, der aus Benutzernamen Namen, Adresse, Alter Handynummer(freiwillig) und E-Mail Adresse. Man kann sich an- und abmelden und sein Profil nachträglich bearbeiten. Im Profil kann eingestellt werden welche Daten öffentlich einsehbar sind</t>
+  </si>
+  <si>
+    <t>Als Nutzer möchte ich Produkte melden können, die illegal sind oder sinnlos sind</t>
+  </si>
+  <si>
+    <t>Produktbild hinzufügen</t>
   </si>
 </sst>
 </file>
@@ -688,21 +699,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="48.6640625" customWidth="1"/>
-    <col min="4" max="4" width="57.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" customWidth="1"/>
+    <col min="5" max="5" width="57.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,374 +721,401 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>67</v>
-      </c>
+      <c r="C4" s="3"/>
       <c r="D4" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3"/>
+      <c r="D5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>79</v>
-      </c>
+      <c r="C8" s="3"/>
       <c r="D8" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="E8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>73</v>
-      </c>
+      <c r="C9" s="3"/>
       <c r="D9" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="C14" s="3"/>
       <c r="D14" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>100</v>
-      </c>
+      <c r="C15" s="3"/>
       <c r="D15" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>93</v>
-      </c>
+      <c r="C16" s="3"/>
       <c r="D16" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E16" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>99</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
       <c r="B19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F21" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E22"/>
+  <autoFilter ref="A1:F22"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1091,15 +1129,15 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="65.33203125" customWidth="1"/>
-    <col min="4" max="4" width="37.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="65.28515625" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1127,13 +1165,13 @@
         <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1144,13 +1182,13 @@
         <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1161,13 +1199,13 @@
         <v>48</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1175,16 +1213,16 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1192,16 +1230,16 @@
         <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1209,16 +1247,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1226,10 +1264,10 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
@@ -1243,10 +1281,10 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E9" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Updated Anforderungen.xlsx Updated Mission.txt
</commit_message>
<xml_diff>
--- a/Anforderungen.xlsx
+++ b/Anforderungen.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="107">
   <si>
     <t>Feature</t>
   </si>
@@ -323,9 +323,6 @@
     <t>Anzeige ob Produkt verfügbar oder nicht</t>
   </si>
   <si>
-    <t>Version</t>
-  </si>
-  <si>
     <t>Bei der ersten Anmeldung muss ein Account angelegt werden, der aus Benutzernamen Namen, Adresse, Alter Handynummer(freiwillig) und E-Mail Adresse. Man kann sich an- und abmelden und sein Profil nachträglich bearbeiten. Im Profil kann eingestellt werden welche Daten öffentlich einsehbar sind</t>
   </si>
   <si>
@@ -333,6 +330,15 @@
   </si>
   <si>
     <t>Produktbild hinzufügen</t>
+  </si>
+  <si>
+    <t>Release</t>
+  </si>
+  <si>
+    <t>Zu jedem auszuleihenden Produkt ein Bild hinzufügen</t>
+  </si>
+  <si>
+    <t>Als Nutzer möchte ich jedem Produkt das ich verleihe ein oder mehrere Bilder hinzufügen um den anderen Benutzern eine bessere Vorstellung des Gegenstandes zu ermöglichen</t>
   </si>
 </sst>
 </file>
@@ -701,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -781,7 +787,7 @@
         <v>66</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>35</v>
@@ -1083,7 +1089,7 @@
         <v>44</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F21" t="s">
         <v>39</v>
@@ -1106,12 +1112,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B23" t="s">
         <v>76</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>